<commit_message>
Art. 84 commi 1 e 2
</commit_message>
<xml_diff>
--- a/camera_pluri.xlsx
+++ b/camera_pluri.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\R\elezioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6724093C-8236-4D65-AFA0-66038203CB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44837B17-556D-4E8A-8D5D-781C6232E65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="15" windowWidth="28830" windowHeight="8850"/>
+    <workbookView xWindow="-105" yWindow="15" windowWidth="28830" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="camera_pluri" sheetId="1" r:id="rId1"/>
@@ -268,12 +268,6 @@
     <t>TOSCANA - 04</t>
   </si>
   <si>
-    <t>TRENTINO-ALTO ADIGE/S_DTIROL</t>
-  </si>
-  <si>
-    <t>TRENTINO-ALTO ADIGE/S_DTIROL - 01</t>
-  </si>
-  <si>
     <t>UMBRIA</t>
   </si>
   <si>
@@ -302,12 +296,18 @@
   </si>
   <si>
     <t>SEGGI</t>
+  </si>
+  <si>
+    <t>TRENTINO-ALTO ADIGE/SÜDTIROL</t>
+  </si>
+  <si>
+    <t>TRENTINO-ALTO ADIGE/SÜDTIROL - 01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1141,11 +1141,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,7 +1162,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1788,10 +1788,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B59" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C59">
         <v>5</v>
@@ -1799,10 +1799,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C60">
         <v>6</v>
@@ -1810,10 +1810,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C61">
         <v>6</v>
@@ -1821,10 +1821,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" t="s">
         <v>86</v>
-      </c>
-      <c r="B62" t="s">
-        <v>88</v>
       </c>
       <c r="C62">
         <v>6</v>
@@ -1832,10 +1832,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B63" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C63">
         <v>6</v>
@@ -1843,10 +1843,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64" t="s">
         <v>89</v>
-      </c>
-      <c r="B64" t="s">
-        <v>91</v>
       </c>
       <c r="C64">
         <v>6</v>
@@ -1854,10 +1854,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C65">
         <v>7</v>

</xml_diff>